<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@8e4a450c507ef6f746e072652acbb72e9504f19a 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ada-tooth-quadrant.xlsx
+++ b/CodeSystem-ada-tooth-quadrant.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>5.0.0</t>
+    <t>6.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,16 +57,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-16T17:36:56+00:00</t>
+    <t>2022-01-21T20:46:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>No display for ContactDetail</t>
+    <t>Alvearie Team</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>United States of America</t>
   </si>
   <si>
     <t>Description</t>
@@ -82,6 +85,9 @@
   </si>
   <si>
     <t>Case Sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Value Set (all codes)</t>
@@ -281,7 +287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -357,94 +363,90 @@
       <c r="A9" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" t="s" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -462,72 +464,72 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@79dae63976c2f2fd3ec2efcb4d3966d843ed4800 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ada-tooth-quadrant.xlsx
+++ b/CodeSystem-ada-tooth-quadrant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>6.0.0</t>
+    <t>6.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-21T20:46:54+00:00</t>
+    <t>2022-05-31T20:10:14+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@11b76e6deee7ca078fcdb804b3d6a01e9ced53fa 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ada-tooth-quadrant.xlsx
+++ b/CodeSystem-ada-tooth-quadrant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>6.1.0</t>
+    <t>6.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-31T20:10:14+00:00</t>
+    <t>2022-06-06T15:56:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@7d4797ac3b571151ee09e452f5ce5095596344c4 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ada-tooth-quadrant.xlsx
+++ b/CodeSystem-ada-tooth-quadrant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>6.1.1</t>
+    <t>7.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-06-06T15:56:40+00:00</t>
+    <t>2022-09-01T20:48:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ LinuxForHealth/alvearie-fhir-ig@80fa500adfae01c9a5dd7ef65e90accc96781b5c 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ada-tooth-quadrant.xlsx
+++ b/CodeSystem-ada-tooth-quadrant.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://ibm.com/fhir/cdm/CodeSystem/ada-tooth-quadrant</t>
+    <t>http://linuxforhealth.org/fhir/cdm/CodeSystem/ada-tooth-quadrant</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>7.0.0</t>
+    <t>8.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,13 +57,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-08T16:11:15+00:00</t>
+    <t>2022-11-10T16:00:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>Alvearie Team</t>
+    <t>LinuxForHealth Team</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>